<commit_message>
baremetrics summary query works
</commit_message>
<xml_diff>
--- a/xls/baremetrics_summary1.xlsx
+++ b/xls/baremetrics_summary1.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="subs" sheetId="1" r:id="rId1"/>
     <sheet name="data" sheetId="3" r:id="rId2"/>
     <sheet name="s2cfg" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="145621" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>query</t>
   </si>
@@ -47,16 +46,37 @@
   </si>
   <si>
     <t>sandbox</t>
+  </si>
+  <si>
+    <t>active_customers</t>
+  </si>
+  <si>
+    <t>arpu</t>
+  </si>
+  <si>
+    <t>arr</t>
+  </si>
+  <si>
+    <t>ltv</t>
+  </si>
+  <si>
+    <t>mrr</t>
+  </si>
+  <si>
+    <t>new_customers</t>
+  </si>
+  <si>
+    <t>user_churn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,16 +105,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
+<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <volType type="realTimeData">
+    <main first="rtdsrv.6ef58dd1ce944dd886df8393ca03ee04">
+      <tp t="s">
+        <v>8</v>
+        <stp/>
+        <stp>baremetrics.summaryQuery1.count</stp>
+        <tr r="B2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.6ef58dd1ce944dd886df8393ca03ee04">
+      <tp t="s">
+        <v>complete</v>
+        <stp/>
+        <stp>baremetrics.summaryQuery1.status</stp>
+        <tr r="B3" s="1"/>
+      </tp>
+    </main>
+  </volType>
+</volTypes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -172,6 +221,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -206,6 +256,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -381,45 +432,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="str">
-        <f ca="1">_xll.s2baremetrics(A1)</f>
+        <f>_xll.s2baremetrics(A1)</f>
         <v>OK</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="e">
-        <f>_xll.s2sub(s2cfg!#REF!,$A$1,A2)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2" t="str">
+        <f>_xll.s2sub(s2cfg!$A$1,$A$1,A2)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="e">
-        <f>_xll.s2sub(s2cfg!#REF!,$A$1,A3)</f>
-        <v>#VALUE!</v>
+      <c r="B3" t="str">
+        <f>_xll.s2sub(s2cfg!$A$1,$A$1,A3)</f>
+        <v>complete</v>
       </c>
     </row>
   </sheetData>
@@ -428,17 +479,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
     <col min="8" max="8" width="13.140625" customWidth="1"/>
@@ -449,49 +504,296 @@
     <col min="13" max="13" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1">
-        <f>_xll.s2tcache( subs!$A$1)</f>
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <f>_xll.s2tcache( subs!$A$1)</f>
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <f>_xll.s2tcache( subs!$A$1)</f>
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <f>_xll.s2tcache( subs!$A$1)</f>
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <f>_xll.s2tcache( subs!$A$1)</f>
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <f>_xll.s2tcache( subs!$A$1)</f>
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <f>_xll.s2tcache( subs!$A$1)</f>
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <f>_xll.s2tcache( subs!$A$1)</f>
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <f>_xll.s2tcache( subs!$A$1)</f>
-        <v>0</v>
-      </c>
-      <c r="J1">
-        <f>_xll.s2tcache( subs!$A$1)</f>
-        <v>0</v>
-      </c>
-      <c r="K1">
-        <f>_xll.s2tcache( subs!$A$1)</f>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="str">
+        <f>_xll.s2today(-7)</f>
+        <v>2017-04-15</v>
+      </c>
+      <c r="C1" s="2" t="str">
+        <f>_xll.s2today(-6)</f>
+        <v>2017-04-16</v>
+      </c>
+      <c r="D1" s="2" t="str">
+        <f>_xll.s2today(-5)</f>
+        <v>2017-04-17</v>
+      </c>
+      <c r="E1" s="2" t="str">
+        <f>_xll.s2today(-4)</f>
+        <v>2017-04-18</v>
+      </c>
+      <c r="F1" s="2" t="str">
+        <f>_xll.s2today(-3)</f>
+        <v>2017-04-19</v>
+      </c>
+      <c r="G1" s="2" t="str">
+        <f>_xll.s2today(-2)</f>
+        <v>2017-04-20</v>
+      </c>
+      <c r="H1" s="2" t="str">
+        <f>_xll.s2today(-1)</f>
+        <v>2017-04-21</v>
+      </c>
+      <c r="I1" s="2" t="str">
+        <f>_xll.s2today(0)</f>
+        <v>2017-04-22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,B$1,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,C$1,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,D$1,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,E$1,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="F2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,F$1,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,G$1,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="H2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,H$1,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,I$1,$A2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,B$1,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="C3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,C$1,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,D$1,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,E$1,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,F$1,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,G$1,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,H$1,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,I$1,$A3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,B$1,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="C4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,C$1,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,D$1,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="E4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,E$1,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,F$1,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="G4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,G$1,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,H$1,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,I$1,$A4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,B$1,$A5)</f>
+        <v>0</v>
+      </c>
+      <c r="C5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,C$1,$A5)</f>
+        <v>0</v>
+      </c>
+      <c r="D5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,D$1,$A5)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,E$1,$A5)</f>
+        <v>0</v>
+      </c>
+      <c r="F5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,F$1,$A5)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,G$1,$A5)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,H$1,$A5)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,I$1,$A5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="str">
+        <f>_xll.s2bcache( subs!$A$1,B$1,$A6)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" t="str">
+        <f>_xll.s2bcache( subs!$A$1,C$1,$A6)</f>
+        <v>0</v>
+      </c>
+      <c r="D6" t="str">
+        <f>_xll.s2bcache( subs!$A$1,D$1,$A6)</f>
+        <v>0</v>
+      </c>
+      <c r="E6" t="str">
+        <f>_xll.s2bcache( subs!$A$1,E$1,$A6)</f>
+        <v>0</v>
+      </c>
+      <c r="F6" t="str">
+        <f>_xll.s2bcache( subs!$A$1,F$1,$A6)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" t="str">
+        <f>_xll.s2bcache( subs!$A$1,G$1,$A6)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" t="str">
+        <f>_xll.s2bcache( subs!$A$1,H$1,$A6)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" t="str">
+        <f>_xll.s2bcache( subs!$A$1,I$1,$A6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="str">
+        <f>_xll.s2bcache( subs!$A$1,B$1,$A7)</f>
+        <v>0</v>
+      </c>
+      <c r="C7" t="str">
+        <f>_xll.s2bcache( subs!$A$1,C$1,$A7)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" t="str">
+        <f>_xll.s2bcache( subs!$A$1,D$1,$A7)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" t="str">
+        <f>_xll.s2bcache( subs!$A$1,E$1,$A7)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" t="str">
+        <f>_xll.s2bcache( subs!$A$1,F$1,$A7)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" t="str">
+        <f>_xll.s2bcache( subs!$A$1,G$1,$A7)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" t="str">
+        <f>_xll.s2bcache( subs!$A$1,H$1,$A7)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" t="str">
+        <f>_xll.s2bcache( subs!$A$1,I$1,$A7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="str">
+        <f>_xll.s2bcache( subs!$A$1,B$1,$A8)</f>
+        <v>0</v>
+      </c>
+      <c r="C8" t="str">
+        <f>_xll.s2bcache( subs!$A$1,C$1,$A8)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" t="str">
+        <f>_xll.s2bcache( subs!$A$1,D$1,$A8)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" t="str">
+        <f>_xll.s2bcache( subs!$A$1,E$1,$A8)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" t="str">
+        <f>_xll.s2bcache( subs!$A$1,F$1,$A8)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" t="str">
+        <f>_xll.s2bcache( subs!$A$1,G$1,$A8)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" t="str">
+        <f>_xll.s2bcache( subs!$A$1,H$1,$A8)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" t="str">
+        <f>_xll.s2bcache( subs!$A$1,I$1,$A8)</f>
         <v>0</v>
       </c>
     </row>
@@ -501,27 +803,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -540,16 +842,16 @@
       <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1">
-        <f ca="1">TODAY()-365</f>
-        <v>42481</v>
+      <c r="G1" s="1" t="str">
+        <f>_xll.s2today(-7)</f>
+        <v>2017-04-15</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1">
-        <f ca="1">TODAY( )</f>
-        <v>42846</v>
+      <c r="I1" s="1" t="str">
+        <f>_xll.s2today( 0)</f>
+        <v>2017-04-22</v>
       </c>
       <c r="J1" t="s">
         <v>9</v>

</xml_diff>